<commit_message>
Dropped a number of variables from the competition case dataset. Most importantly, I have removed all work on the deterrence threshold. Also, I have dropped a few intermediate results from the compCase.RData, but that could be easily undone.
</commit_message>
<xml_diff>
--- a/inputData/DgComp/case_data_codebook.xlsx
+++ b/inputData/DgComp/case_data_codebook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="27915" windowHeight="16440"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="27920" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>mkt</t>
   </si>
@@ -54,12 +54,6 @@
     <t>Calculation</t>
   </si>
   <si>
-    <t>SBS 2014</t>
-  </si>
-  <si>
-    <t>Assumed deterrence threshold</t>
-  </si>
-  <si>
     <t>Size of the market affected by case "k" in millions of euros</t>
   </si>
   <si>
@@ -81,27 +75,12 @@
     <t>Estimated gross output at the four digit NACE2 level associated with case "k" in sector "i" based on the 64 sector aggregation</t>
   </si>
   <si>
-    <t>Estimated size of the market affected by case "k" including deterrent effects based on the 64 sector aggregation</t>
-  </si>
-  <si>
-    <t>Contribution to the shock including deterrent effects of case "k" with respect to the overall economy based on the 64 sector aggregation</t>
-  </si>
-  <si>
-    <t>Contribution to the shock including deterrent effects of case "k" with respect to the overall economy based on the 24 sector aggregation</t>
-  </si>
-  <si>
-    <t>Estimated size of the market affected by case "k" including deterrent effects based on the 24 sector aggregation</t>
-  </si>
-  <si>
     <t>Estimated gross output at the four digit NACE2 level associated with case "k" in sector "i" based on the 24 sector aggregation</t>
   </si>
   <si>
     <t>Gross output at the two digit NACE2 level associated with sector "i" based on the 24 sector aggregation</t>
   </si>
   <si>
-    <t>Contribution to the shock including deterrent effects of case "k" according to a logistic function for deterrence with respect to the overall economy based on the 64 sector aggregation</t>
-  </si>
-  <si>
     <t>case_id</t>
   </si>
   <si>
@@ -117,9 +96,6 @@
     <t>delta_p</t>
   </si>
   <si>
-    <t>thr</t>
-  </si>
-  <si>
     <t>nace2_4d</t>
   </si>
   <si>
@@ -132,15 +108,6 @@
     <t>mup_a24</t>
   </si>
   <si>
-    <t>prod4</t>
-  </si>
-  <si>
-    <t>prod2_a64</t>
-  </si>
-  <si>
-    <t>prod2_a24</t>
-  </si>
-  <si>
     <t>go2_a64</t>
   </si>
   <si>
@@ -162,121 +129,31 @@
     <t>go</t>
   </si>
   <si>
-    <t>delta_mup_a64</t>
-  </si>
-  <si>
-    <t>delta_mup_a24</t>
-  </si>
-  <si>
-    <t>delta_mup_a64_log</t>
-  </si>
-  <si>
-    <t>go4_a64_prod</t>
-  </si>
-  <si>
-    <t>go4_a24_prod</t>
-  </si>
-  <si>
-    <t>va4</t>
-  </si>
-  <si>
-    <t>va2_a64</t>
-  </si>
-  <si>
-    <t>va2_a24</t>
-  </si>
-  <si>
-    <t>go4_a64_va</t>
-  </si>
-  <si>
-    <t>go4_a24_va</t>
-  </si>
-  <si>
-    <t>n4_a64</t>
-  </si>
-  <si>
-    <t>n4_a24</t>
-  </si>
-  <si>
     <t>Variable name</t>
   </si>
   <si>
-    <t>go4_a64_prod = ( prod4 / prod2_a64 ) * go2_a64</t>
-  </si>
-  <si>
-    <t>go4_a24_prod = ( prod4 / prod2_a24 ) * go2_a24</t>
-  </si>
-  <si>
-    <t>go4_a64_n = go2_a64 / n4_a64</t>
-  </si>
-  <si>
-    <t>go4_a24_n = go2_a24 / n4_a24</t>
-  </si>
-  <si>
-    <t>Value added at the four digit NACE2 level</t>
-  </si>
-  <si>
     <t>Documents how go4_a64 is estimated. It takes one of three values: go4_a64_prod (production value), go4_a64_va (value added), or go4_a64_n (number of NACE2 classes). See the comments on the corresponding variables (below).</t>
   </si>
   <si>
     <t>Documents how go4_a64 is estimated. It takes one of three values: go4_a24_prod (production value), go4_a24_va (valued added), or go4_a24_n (number of NACE2 classes). See the comments on the corresponding variables (below).</t>
   </si>
   <si>
-    <t>Value added at the two digit NACE2 level based on the 64 sector aggregation</t>
-  </si>
-  <si>
-    <t>Value added at the two digit NACE2 level based on the 24 sector aggregation</t>
-  </si>
-  <si>
-    <t>Number of NACE2 classes (i.e. 4-digit codes) in the relevant A64 aggregate</t>
-  </si>
-  <si>
-    <t>Number of NACE2 classes (i.e. 4-digit codes) in the relevant A24 aggregate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">go4_a64_va = ( va4 / va2_a64 ) * go2_a64 </t>
-  </si>
-  <si>
-    <t>go4_a24_va = ( va4 / va2_a24 ) * go2_a24</t>
-  </si>
-  <si>
-    <t>NACE Rev. 2</t>
-  </si>
-  <si>
-    <t>go4_a64_n4</t>
-  </si>
-  <si>
-    <t>go4_a24_n4</t>
-  </si>
-  <si>
     <t>Gross output of the entire economy which is does not depend on the aggregation that is used (A64 or A24). Only accounts for the "business economy", i.e., those industries that appear in the Ecfin dataset</t>
   </si>
   <si>
     <t>Label</t>
   </si>
   <si>
-    <t>mkt_t_a64_log</t>
-  </si>
-  <si>
-    <t>mkt_t_a24</t>
-  </si>
-  <si>
-    <t>mkt_t_a64</t>
-  </si>
-  <si>
-    <t>Production value at the four digit NACE2 level (refer to report for imputation rules)</t>
-  </si>
-  <si>
-    <t>SBS</t>
-  </si>
-  <si>
-    <t>Production value at the two digit NACE2 level based on the 64 sector aggregation (refer to report for imputation rules)</t>
-  </si>
-  <si>
-    <t>Production value at the two digit NACE2 level based on the 24 sector aggregation (refer to report for imputation rules)</t>
-  </si>
-  <si>
-    <t>Estimated size of the market affectet by case "k" including deterrent effects according to a logistic function based on the 64 sector aggregation. [Logistic parameters: chi = 100, ef = .0154 (cartels) and .0254 (mergers), ny = 1]</t>
+    <t>mktT</t>
+  </si>
+  <si>
+    <t>mktD</t>
+  </si>
+  <si>
+    <t>Estimated size of the market deterred by the decision on case "k". Deterrent effects are calculated according to a logistic function based on the 64 sector aggregation. [Logistic parameters: chi = 100, ef = .0154 (cartels) and .0254 (mergers), ny = 1]</t>
+  </si>
+  <si>
+    <t>mkT = mkt + mktD</t>
   </si>
 </sst>
 </file>
@@ -355,7 +232,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="82">
+  <cellStyleXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -438,8 +315,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -463,8 +360,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="82">
+  <cellStyles count="102">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -505,6 +406,16 @@
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -545,6 +456,16 @@
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -845,34 +766,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E39"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="60.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>7</v>
@@ -881,11 +800,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>7</v>
@@ -894,11 +812,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>7</v>
@@ -907,457 +824,194 @@
         <v>3</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" ht="42">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" s="10" customFormat="1" ht="56">
       <c r="A8" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" ht="28">
       <c r="A14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" ht="28">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" ht="56">
+      <c r="A16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" ht="28">
       <c r="A17" s="5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" ht="28">
       <c r="A18" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" ht="56">
       <c r="A19" s="5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="7" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" ht="42">
       <c r="A20" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Separated dataset merge, go4 estimation, logistic deterrence and dataset formatting into separate scripts. Fixed more nace2 code issues in cleanCompData.R.
</commit_message>
<xml_diff>
--- a/inputData/DgComp/case_data_codebook.xlsx
+++ b/inputData/DgComp/case_data_codebook.xlsx
@@ -132,12 +132,6 @@
     <t>Variable name</t>
   </si>
   <si>
-    <t>Documents how go4_a64 is estimated. It takes one of three values: go4_a64_prod (production value), go4_a64_va (value added), or go4_a64_n (number of NACE2 classes). See the comments on the corresponding variables (below).</t>
-  </si>
-  <si>
-    <t>Documents how go4_a64 is estimated. It takes one of three values: go4_a24_prod (production value), go4_a24_va (valued added), or go4_a24_n (number of NACE2 classes). See the comments on the corresponding variables (below).</t>
-  </si>
-  <si>
     <t>Gross output of the entire economy which is does not depend on the aggregation that is used (A64 or A24). Only accounts for the "business economy", i.e., those industries that appear in the Ecfin dataset</t>
   </si>
   <si>
@@ -154,6 +148,12 @@
   </si>
   <si>
     <t>mkT = mkt + mktD</t>
+  </si>
+  <si>
+    <t>Documents how go4_a64 is estimated. It takes one of three values: go4_a64_prod (production value), go4_a64_va (value added), or go4_a64_n (number of NACE2 classes)</t>
+  </si>
+  <si>
+    <t>Documents how go4_a64 is estimated. It takes one of three values: go4_a24_prod (production value), go4_a24_va (valued added), or go4_a24_n (number of NACE2 classes)</t>
   </si>
 </sst>
 </file>
@@ -232,9 +232,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="102">
+  <cellStyleXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -365,7 +369,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="102">
+  <cellStyles count="106">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -416,6 +420,8 @@
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -466,6 +472,8 @@
     <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -769,7 +777,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -786,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -825,75 +835,75 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="42">
+    <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="42">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" s="10" customFormat="1" ht="56">
-      <c r="A8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" s="10" customFormat="1" ht="56">
       <c r="A9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -911,59 +921,59 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="28">
       <c r="A13" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" ht="28">
       <c r="A14" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="28">
+    <row r="15" spans="1:4" ht="42">
       <c r="A15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="56">
+    <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="C16" s="7" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -991,13 +1001,13 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="56">
+    <row r="19" spans="1:4" ht="42">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1009,7 +1019,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated analysis for 2020 final report
</commit_message>
<xml_diff>
--- a/inputData/DgComp/case_data_codebook.xlsx
+++ b/inputData/DgComp/case_data_codebook.xlsx
@@ -144,9 +144,6 @@
     <t>mktD</t>
   </si>
   <si>
-    <t>Estimated size of the market deterred by the decision on case "k". Deterrent effects are calculated according to a logistic function based on the 64 sector aggregation. [Logistic parameters: chi = 100, ef = .0154 (cartels) and .0254 (mergers), ny = 1]</t>
-  </si>
-  <si>
     <t>mkT = mkt + mktD</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Documents how go4_a64 is estimated. It takes one of three values: go4_a24_prod (production value), go4_a24_va (valued added), or go4_a24_n (number of NACE2 classes)</t>
+  </si>
+  <si>
+    <t>Estimated size of the market deterred by the decision on case "k". Deterrent effects are calculated according to a logistic function based on the 64 sector aggregation. [Logistic parameters: chi = 100, ef = .014891 (cartels) and .025906 (mergers), ny = 1]</t>
   </si>
 </sst>
 </file>
@@ -777,8 +777,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -891,7 +891,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D9" s="9"/>
     </row>
@@ -903,7 +903,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -961,7 +961,7 @@
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1"/>
     </row>

</xml_diff>